<commit_message>
completed hyperparameter tuning and produce graph nn results
</commit_message>
<xml_diff>
--- a/Data/Predictions/Graph Neural Network/Inductive/exclude_previous_rating_model_1_predictions.xlsx
+++ b/Data/Predictions/Graph Neural Network/Inductive/exclude_previous_rating_model_1_predictions.xlsx
@@ -509,7 +509,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -815,7 +815,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -917,7 +917,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1359,7 +1359,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -1886,7 +1886,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2090,7 +2090,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2345,7 +2345,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2515,7 +2515,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2532,7 +2532,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -2617,7 +2617,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -2634,7 +2634,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -2651,7 +2651,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -2719,7 +2719,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -2940,7 +2940,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -3042,7 +3042,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -3076,7 +3076,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -3093,7 +3093,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -3212,7 +3212,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -3229,7 +3229,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -3246,7 +3246,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -3263,7 +3263,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -3348,7 +3348,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -3382,7 +3382,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -3399,7 +3399,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -3416,7 +3416,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -3484,7 +3484,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -3518,7 +3518,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -3535,7 +3535,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -3637,7 +3637,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -3739,7 +3739,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -3756,7 +3756,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -3807,7 +3807,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -3943,7 +3943,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -3977,7 +3977,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -4045,7 +4045,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -4062,7 +4062,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -4147,7 +4147,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -4164,7 +4164,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -4181,7 +4181,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -4198,7 +4198,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -4232,7 +4232,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -4300,7 +4300,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -4317,7 +4317,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -4470,7 +4470,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -4708,7 +4708,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -4776,7 +4776,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -4810,7 +4810,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
@@ -4827,7 +4827,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -4844,7 +4844,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -4878,7 +4878,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -4946,7 +4946,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -4963,7 +4963,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -5014,7 +5014,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -5031,7 +5031,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -5065,7 +5065,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -5082,7 +5082,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -5099,7 +5099,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -5167,7 +5167,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -5320,7 +5320,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -5405,7 +5405,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -5439,7 +5439,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -5456,7 +5456,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -5541,7 +5541,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -5609,7 +5609,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -5626,7 +5626,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -5643,7 +5643,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -5660,7 +5660,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -5677,7 +5677,7 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -5694,7 +5694,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -5762,7 +5762,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -5779,7 +5779,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -5830,7 +5830,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -5915,7 +5915,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -5949,7 +5949,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -5983,7 +5983,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -6034,7 +6034,7 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>AAA</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -6068,7 +6068,7 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -6085,7 +6085,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
@@ -6153,7 +6153,7 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
@@ -6187,7 +6187,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
@@ -6204,7 +6204,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
@@ -6272,7 +6272,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
@@ -6306,7 +6306,7 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
@@ -6323,7 +6323,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
@@ -6374,7 +6374,7 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
@@ -6408,7 +6408,7 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
@@ -6493,7 +6493,7 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
@@ -6561,7 +6561,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
@@ -6629,7 +6629,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
@@ -6646,7 +6646,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
@@ -6663,7 +6663,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
@@ -6714,7 +6714,7 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
@@ -6850,7 +6850,7 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
@@ -6867,7 +6867,7 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
@@ -6884,7 +6884,7 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
@@ -6901,7 +6901,7 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
@@ -6918,7 +6918,7 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
@@ -6952,7 +6952,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
@@ -7020,7 +7020,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
@@ -7037,7 +7037,7 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
@@ -7088,7 +7088,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
@@ -7156,7 +7156,7 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
@@ -7173,7 +7173,7 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
@@ -7190,7 +7190,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
@@ -7207,7 +7207,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
@@ -7224,7 +7224,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
@@ -7275,7 +7275,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">

</xml_diff>

<commit_message>
revamp gnn dataset and add statistical tests
</commit_message>
<xml_diff>
--- a/Data/Predictions/Graph Neural Network/Inductive/exclude_previous_rating_model_1_predictions.xlsx
+++ b/Data/Predictions/Graph Neural Network/Inductive/exclude_previous_rating_model_1_predictions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C403"/>
+  <dimension ref="A1:C402"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -662,7 +662,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2243,7 +2243,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2532,7 +2532,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -3076,7 +3076,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -3093,7 +3093,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3246,7 +3246,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -3348,7 +3348,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -3365,7 +3365,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -3382,7 +3382,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -3518,7 +3518,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -3734,7 +3734,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -3744,14 +3744,14 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>KODK : 2016-10-01</t>
+          <t>KOS : 2016-01-01</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>CCC</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -3761,7 +3761,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>KOS : 2016-01-01</t>
+          <t>KSS : 2013-07-01</t>
         </is>
       </c>
     </row>
@@ -3778,14 +3778,14 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>KSS : 2013-07-01</t>
+          <t>KSS : 2014-10-01</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -3795,14 +3795,14 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>KSS : 2014-10-01</t>
+          <t>KW : 2015-01-01</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -3812,7 +3812,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>KW : 2015-01-01</t>
+          <t>LAMR : 2015-07-01</t>
         </is>
       </c>
     </row>
@@ -3829,7 +3829,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>LAMR : 2015-07-01</t>
+          <t>LAMR : 2016-04-01</t>
         </is>
       </c>
     </row>
@@ -3846,14 +3846,14 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>LAMR : 2016-04-01</t>
+          <t>LKQ : 2016-04-01</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -3863,14 +3863,14 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>LKQ : 2016-04-01</t>
+          <t>LLY : 2012-01-01</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>AAA</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -3880,7 +3880,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>LLY : 2012-01-01</t>
+          <t>LLY : 2015-04-01</t>
         </is>
       </c>
     </row>
@@ -3897,14 +3897,14 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>LLY : 2015-04-01</t>
+          <t>LLY : 2015-10-01</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>AAA</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -3914,14 +3914,14 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>LLY : 2015-10-01</t>
+          <t>LPX : 2014-10-01</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -3931,7 +3931,7 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>LPX : 2014-10-01</t>
+          <t>LRCX : 2013-07-01</t>
         </is>
       </c>
     </row>
@@ -3948,7 +3948,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>LRCX : 2013-07-01</t>
+          <t>LUV : 2012-04-01</t>
         </is>
       </c>
     </row>
@@ -3965,7 +3965,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>LUV : 2012-04-01</t>
+          <t>LUV : 2013-10-01</t>
         </is>
       </c>
     </row>
@@ -3982,7 +3982,7 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>LUV : 2013-10-01</t>
+          <t>LUV : 2014-07-01</t>
         </is>
       </c>
     </row>
@@ -3999,7 +3999,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>LUV : 2014-07-01</t>
+          <t>LUV : 2014-10-01</t>
         </is>
       </c>
     </row>
@@ -4016,14 +4016,14 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>LUV : 2014-10-01</t>
+          <t>LVS : 2015-04-01</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -4033,24 +4033,24 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>LVS : 2015-04-01</t>
+          <t>LYV : 2016-07-01</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>LYV : 2016-07-01</t>
+          <t>MCHP : 2012-10-01</t>
         </is>
       </c>
     </row>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>MCHP : 2012-10-01</t>
+          <t>MCHP : 2013-01-01</t>
         </is>
       </c>
     </row>
@@ -4079,19 +4079,19 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>MCHP : 2013-01-01</t>
+          <t>MCHP : 2015-01-01</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -4101,14 +4101,14 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>MCHP : 2015-01-01</t>
+          <t>MCHP : 2015-04-01</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -4118,14 +4118,14 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>MCHP : 2015-04-01</t>
+          <t>MCHP : 2016-04-01</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -4135,7 +4135,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>MCHP : 2016-04-01</t>
+          <t>MCO : 2012-07-01</t>
         </is>
       </c>
     </row>
@@ -4152,7 +4152,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>MCO : 2012-07-01</t>
+          <t>MCO : 2013-01-01</t>
         </is>
       </c>
     </row>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>MCO : 2013-01-01</t>
+          <t>MCO : 2014-01-01</t>
         </is>
       </c>
     </row>
@@ -4186,7 +4186,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>MCO : 2014-01-01</t>
+          <t>MCO : 2014-07-01</t>
         </is>
       </c>
     </row>
@@ -4198,12 +4198,12 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>MCO : 2014-07-01</t>
+          <t>MCO : 2015-04-01</t>
         </is>
       </c>
     </row>
@@ -4215,19 +4215,19 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>MCO : 2015-04-01</t>
+          <t>MCO : 2015-10-01</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -4237,14 +4237,14 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>MCO : 2015-10-01</t>
+          <t>MDLZ : 2012-04-01</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>MDLZ : 2012-04-01</t>
+          <t>MDLZ : 2012-10-01</t>
         </is>
       </c>
     </row>
@@ -4271,7 +4271,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>MDLZ : 2012-10-01</t>
+          <t>MDLZ : 2016-04-01</t>
         </is>
       </c>
     </row>
@@ -4288,14 +4288,14 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>MDLZ : 2016-04-01</t>
+          <t>MEOH : 2016-10-01</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -4305,14 +4305,14 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>MEOH : 2016-10-01</t>
+          <t>MERC : 2016-01-01</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -4322,14 +4322,14 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>MERC : 2016-01-01</t>
+          <t>MGM : 2014-07-01</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>CCC</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -4339,7 +4339,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>MGM : 2014-07-01</t>
+          <t>MLM : 2013-07-01</t>
         </is>
       </c>
     </row>
@@ -4356,48 +4356,48 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>MLM : 2013-07-01</t>
+          <t>MLM : 2016-10-01</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>MLM : 2016-10-01</t>
+          <t>MMM : 2015-04-01</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>MMM : 2015-04-01</t>
+          <t>MMP : 2013-04-01</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -4407,14 +4407,14 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>MMP : 2013-04-01</t>
+          <t>MMP : 2014-07-01</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -4424,14 +4424,14 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>MMP : 2014-07-01</t>
+          <t>MMP : 2016-07-01</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -4441,14 +4441,14 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>MMP : 2016-07-01</t>
+          <t>MRC : 2014-07-01</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -4458,14 +4458,14 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>MRC : 2014-07-01</t>
+          <t>MRC : 2015-07-01</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>AAA</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -4475,7 +4475,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>MRC : 2015-07-01</t>
+          <t>MRK : 2015-10-01</t>
         </is>
       </c>
     </row>
@@ -4492,7 +4492,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>MRK : 2015-10-01</t>
+          <t>MRK : 2016-01-01</t>
         </is>
       </c>
     </row>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>MRK : 2016-01-01</t>
+          <t>MSFT : 2011-10-01</t>
         </is>
       </c>
     </row>
@@ -4521,12 +4521,12 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>MSFT : 2011-10-01</t>
+          <t>MSFT : 2013-10-01</t>
         </is>
       </c>
     </row>
@@ -4543,24 +4543,24 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>MSFT : 2013-10-01</t>
+          <t>MSFT : 2014-01-01</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>AAA</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>MSFT : 2014-01-01</t>
+          <t>MSI : 2011-10-01</t>
         </is>
       </c>
     </row>
@@ -4577,7 +4577,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>MSI : 2011-10-01</t>
+          <t>MSI : 2012-07-01</t>
         </is>
       </c>
     </row>
@@ -4594,7 +4594,7 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>MSI : 2012-07-01</t>
+          <t>MSI : 2013-01-01</t>
         </is>
       </c>
     </row>
@@ -4611,7 +4611,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>MSI : 2013-01-01</t>
+          <t>MSI : 2013-04-01</t>
         </is>
       </c>
     </row>
@@ -4628,7 +4628,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>MSI : 2013-04-01</t>
+          <t>MSI : 2013-07-01</t>
         </is>
       </c>
     </row>
@@ -4645,14 +4645,14 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>MSI : 2013-07-01</t>
+          <t>MSI : 2015-01-01</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -4662,7 +4662,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>MSI : 2015-01-01</t>
+          <t>MTN : 2016-01-01</t>
         </is>
       </c>
     </row>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>MTN : 2016-01-01</t>
+          <t>MTZ : 2012-07-01</t>
         </is>
       </c>
     </row>
@@ -4696,7 +4696,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>MTZ : 2012-07-01</t>
+          <t>MTZ : 2015-01-01</t>
         </is>
       </c>
     </row>
@@ -4713,7 +4713,7 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>MTZ : 2015-01-01</t>
+          <t>MUR : 2015-01-01</t>
         </is>
       </c>
     </row>
@@ -4730,7 +4730,7 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>MUR : 2015-01-01</t>
+          <t>NCR : 2015-04-01</t>
         </is>
       </c>
     </row>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>NCR : 2015-04-01</t>
+          <t>NCR : 2015-10-01</t>
         </is>
       </c>
     </row>
@@ -4764,7 +4764,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>NCR : 2015-10-01</t>
+          <t>NCR : 2016-04-01</t>
         </is>
       </c>
     </row>
@@ -4781,14 +4781,14 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>NCR : 2016-04-01</t>
+          <t>NCR : 2016-07-01</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -4798,7 +4798,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>NCR : 2016-07-01</t>
+          <t>NEE : 2012-01-01</t>
         </is>
       </c>
     </row>
@@ -4815,7 +4815,7 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>NEE : 2012-01-01</t>
+          <t>NEE : 2012-04-01</t>
         </is>
       </c>
     </row>
@@ -4832,7 +4832,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>NEE : 2012-04-01</t>
+          <t>NEE : 2012-10-01</t>
         </is>
       </c>
     </row>
@@ -4849,14 +4849,14 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>NEE : 2012-10-01</t>
+          <t>NEM : 2014-04-01</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -4866,14 +4866,14 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>NEM : 2014-04-01</t>
+          <t>NFG : 2015-01-01</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -4883,14 +4883,14 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>NFG : 2015-01-01</t>
+          <t>NFLX : 2013-10-01</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -4900,14 +4900,14 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>NFLX : 2013-10-01</t>
+          <t>NFLX : 2015-10-01</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -4917,7 +4917,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>NFLX : 2015-10-01</t>
+          <t>NGL : 2015-01-01</t>
         </is>
       </c>
     </row>
@@ -4934,14 +4934,14 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>NGL : 2015-01-01</t>
+          <t>NGL : 2016-10-01</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -4951,7 +4951,7 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>NGL : 2016-10-01</t>
+          <t>NOC : 2012-07-01</t>
         </is>
       </c>
     </row>
@@ -4968,7 +4968,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>NOC : 2012-07-01</t>
+          <t>NOC : 2016-01-01</t>
         </is>
       </c>
     </row>
@@ -4985,14 +4985,14 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>NOC : 2016-01-01</t>
+          <t>NOC : 2016-07-01</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -5002,7 +5002,7 @@
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>NOC : 2016-07-01</t>
+          <t>NRG : 2014-07-01</t>
         </is>
       </c>
     </row>
@@ -5019,14 +5019,14 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>NRG : 2014-07-01</t>
+          <t>NRG : 2016-01-01</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -5036,14 +5036,14 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>NRG : 2016-01-01</t>
+          <t>NTAP : 2014-07-01</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -5053,14 +5053,14 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>NTAP : 2014-07-01</t>
+          <t>NVDA : 2015-10-01</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -5070,14 +5070,14 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>NVDA : 2015-10-01</t>
+          <t>NWE : 2014-07-01</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -5087,14 +5087,14 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>NWE : 2014-07-01</t>
+          <t>OGE : 2016-04-01</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -5104,14 +5104,14 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>OGE : 2016-04-01</t>
+          <t>OLN : 2015-07-01</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -5121,7 +5121,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>OLN : 2015-07-01</t>
+          <t>ORCL : 2012-07-01</t>
         </is>
       </c>
     </row>
@@ -5138,7 +5138,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>ORCL : 2012-07-01</t>
+          <t>ORCL : 2013-10-01</t>
         </is>
       </c>
     </row>
@@ -5155,7 +5155,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>ORCL : 2013-10-01</t>
+          <t>ORCL : 2014-01-01</t>
         </is>
       </c>
     </row>
@@ -5172,7 +5172,7 @@
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>ORCL : 2014-01-01</t>
+          <t>ORCL : 2015-04-01</t>
         </is>
       </c>
     </row>
@@ -5189,7 +5189,7 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>ORCL : 2015-04-01</t>
+          <t>ORCL : 2016-01-01</t>
         </is>
       </c>
     </row>
@@ -5201,19 +5201,19 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>ORCL : 2016-01-01</t>
+          <t>ORCL : 2016-10-01</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -5223,7 +5223,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>ORCL : 2016-10-01</t>
+          <t>ORLY : 2014-04-01</t>
         </is>
       </c>
     </row>
@@ -5240,7 +5240,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>ORLY : 2014-04-01</t>
+          <t>OTEX : 2014-01-01</t>
         </is>
       </c>
     </row>
@@ -5257,14 +5257,14 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>OTEX : 2014-01-01</t>
+          <t>OTEX : 2015-01-01</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -5274,14 +5274,14 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>OTEX : 2015-01-01</t>
+          <t>OTEX : 2015-10-01</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -5291,14 +5291,14 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>OTEX : 2015-10-01</t>
+          <t>OXY : 2014-07-01</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -5308,14 +5308,14 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>OXY : 2014-07-01</t>
+          <t>PAA : 2015-01-01</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -5325,14 +5325,14 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>PAA : 2015-01-01</t>
+          <t>PAG : 2015-10-01</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -5342,7 +5342,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>PAG : 2015-10-01</t>
+          <t>PBI : 2012-10-01</t>
         </is>
       </c>
     </row>
@@ -5359,7 +5359,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>PBI : 2012-10-01</t>
+          <t>PCAR : 2016-04-01</t>
         </is>
       </c>
     </row>
@@ -5376,14 +5376,14 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>PCAR : 2016-04-01</t>
+          <t>PCAR : 2016-07-01</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -5393,24 +5393,24 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>PCAR : 2016-07-01</t>
+          <t>PCG : 2013-04-01</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>PCG : 2013-04-01</t>
+          <t>PCG : 2015-07-01</t>
         </is>
       </c>
     </row>
@@ -5422,12 +5422,12 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>PCG : 2015-07-01</t>
+          <t>PEG : 2013-10-01</t>
         </is>
       </c>
     </row>
@@ -5444,7 +5444,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>PEG : 2013-10-01</t>
+          <t>PEG : 2014-07-01</t>
         </is>
       </c>
     </row>
@@ -5461,7 +5461,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>PEG : 2014-07-01</t>
+          <t>PEG : 2014-10-01</t>
         </is>
       </c>
     </row>
@@ -5478,7 +5478,7 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>PEG : 2014-10-01</t>
+          <t>PEG : 2015-01-01</t>
         </is>
       </c>
     </row>
@@ -5495,7 +5495,7 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>PEG : 2015-01-01</t>
+          <t>PEG : 2015-10-01</t>
         </is>
       </c>
     </row>
@@ -5512,7 +5512,7 @@
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>PEG : 2015-10-01</t>
+          <t>PEP : 2014-04-01</t>
         </is>
       </c>
     </row>
@@ -5529,7 +5529,7 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>PEP : 2014-04-01</t>
+          <t>PEP : 2015-01-01</t>
         </is>
       </c>
     </row>
@@ -5546,7 +5546,7 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>PEP : 2015-01-01</t>
+          <t>PEP : 2015-10-01</t>
         </is>
       </c>
     </row>
@@ -5563,14 +5563,14 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>PEP : 2015-10-01</t>
+          <t>PEP : 2016-01-01</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
@@ -5580,7 +5580,7 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>PEP : 2016-01-01</t>
+          <t>PFGC : 2016-10-01</t>
         </is>
       </c>
     </row>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>PFGC : 2016-10-01</t>
+          <t>PNM : 2012-04-01</t>
         </is>
       </c>
     </row>
@@ -5609,19 +5609,19 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>PNM : 2012-04-01</t>
+          <t>PNM : 2013-10-01</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -5631,7 +5631,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>PNM : 2013-10-01</t>
+          <t>PNW : 2016-07-01</t>
         </is>
       </c>
     </row>
@@ -5648,7 +5648,7 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>PNW : 2016-07-01</t>
+          <t>POR : 2012-10-01</t>
         </is>
       </c>
     </row>
@@ -5665,14 +5665,14 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>POR : 2012-10-01</t>
+          <t>POR : 2014-01-01</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -5682,14 +5682,14 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>POR : 2014-01-01</t>
+          <t>POST : 2016-04-01</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -5699,7 +5699,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>POST : 2016-04-01</t>
+          <t>PSX : 2016-07-01</t>
         </is>
       </c>
     </row>
@@ -5716,14 +5716,14 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>PSX : 2016-07-01</t>
+          <t>PSX : 2016-10-01</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
@@ -5733,14 +5733,14 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>PSX : 2016-10-01</t>
+          <t>PXD : 2012-07-01</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
@@ -5750,14 +5750,14 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>PXD : 2012-07-01</t>
+          <t>RHP : 2014-04-01</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
@@ -5767,7 +5767,7 @@
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>RHP : 2014-04-01</t>
+          <t>RRC : 2012-04-01</t>
         </is>
       </c>
     </row>
@@ -5784,7 +5784,7 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>RRC : 2012-04-01</t>
+          <t>RRC : 2014-10-01</t>
         </is>
       </c>
     </row>
@@ -5801,7 +5801,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>RRC : 2014-10-01</t>
+          <t>RRC : 2015-10-01</t>
         </is>
       </c>
     </row>
@@ -5818,14 +5818,14 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>RRC : 2015-10-01</t>
+          <t>RRC : 2016-10-01</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
@@ -5835,7 +5835,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>RRC : 2016-10-01</t>
+          <t>RS : 2014-04-01</t>
         </is>
       </c>
     </row>
@@ -5852,7 +5852,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>RS : 2014-04-01</t>
+          <t>RS : 2016-01-01</t>
         </is>
       </c>
     </row>
@@ -5869,7 +5869,7 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>RS : 2016-01-01</t>
+          <t>RS : 2016-04-01</t>
         </is>
       </c>
     </row>
@@ -5886,24 +5886,24 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>RS : 2016-04-01</t>
+          <t>RS : 2016-07-01</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>RS : 2016-07-01</t>
+          <t>SALM : 2016-01-01</t>
         </is>
       </c>
     </row>
@@ -5915,12 +5915,12 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>SALM : 2016-01-01</t>
+          <t>SALM : 2016-04-01</t>
         </is>
       </c>
     </row>
@@ -5932,12 +5932,12 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>SALM : 2016-04-01</t>
+          <t>SBAC : 2016-04-01</t>
         </is>
       </c>
     </row>
@@ -5949,12 +5949,12 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>SBAC : 2016-04-01</t>
+          <t>SBGI : 2015-07-01</t>
         </is>
       </c>
     </row>
@@ -5966,29 +5966,29 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>SBGI : 2015-07-01</t>
+          <t>SBGI : 2015-10-01</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>SBGI : 2015-10-01</t>
+          <t>SBUX : 2012-10-01</t>
         </is>
       </c>
     </row>
@@ -6005,7 +6005,7 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>SBUX : 2012-10-01</t>
+          <t>SBUX : 2015-04-01</t>
         </is>
       </c>
     </row>
@@ -6022,7 +6022,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>SBUX : 2015-04-01</t>
+          <t>SBUX : 2016-07-01</t>
         </is>
       </c>
     </row>
@@ -6039,14 +6039,14 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>SBUX : 2016-07-01</t>
+          <t>SCCO : 2016-10-01</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -6056,7 +6056,7 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>SCCO : 2016-10-01</t>
+          <t>SEAS : 2016-04-01</t>
         </is>
       </c>
     </row>
@@ -6073,14 +6073,14 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>SEAS : 2016-04-01</t>
+          <t>SLCA : 2014-10-01</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -6090,14 +6090,14 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>SLCA : 2014-10-01</t>
+          <t>SLCA : 2016-10-01</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -6107,7 +6107,7 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>SLCA : 2016-10-01</t>
+          <t>SLGN : 2016-07-01</t>
         </is>
       </c>
     </row>
@@ -6124,7 +6124,7 @@
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>SLGN : 2016-07-01</t>
+          <t>SM : 2014-10-01</t>
         </is>
       </c>
     </row>
@@ -6141,14 +6141,14 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>SM : 2014-10-01</t>
+          <t>SM : 2015-10-01</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -6158,14 +6158,14 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>SM : 2015-10-01</t>
+          <t>SNA : 2014-04-01</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
@@ -6175,7 +6175,7 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>SNA : 2014-04-01</t>
+          <t>SRE : 2013-07-01</t>
         </is>
       </c>
     </row>
@@ -6192,14 +6192,14 @@
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>SRE : 2013-07-01</t>
+          <t>SRE : 2016-04-01</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -6209,7 +6209,7 @@
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>SRE : 2016-04-01</t>
+          <t>SSP : 2015-04-01</t>
         </is>
       </c>
     </row>
@@ -6226,7 +6226,7 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>SSP : 2015-04-01</t>
+          <t>SSP : 2016-07-01</t>
         </is>
       </c>
     </row>
@@ -6243,7 +6243,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>SSP : 2016-07-01</t>
+          <t>STLD : 2016-10-01</t>
         </is>
       </c>
     </row>
@@ -6260,7 +6260,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>STLD : 2016-10-01</t>
+          <t>STX : 2013-07-01</t>
         </is>
       </c>
     </row>
@@ -6277,7 +6277,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>STX : 2013-07-01</t>
+          <t>STX : 2013-10-01</t>
         </is>
       </c>
     </row>
@@ -6294,7 +6294,7 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>STX : 2013-10-01</t>
+          <t>STX : 2014-07-01</t>
         </is>
       </c>
     </row>
@@ -6311,7 +6311,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>STX : 2014-07-01</t>
+          <t>STX : 2015-04-01</t>
         </is>
       </c>
     </row>
@@ -6328,14 +6328,14 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>STX : 2015-04-01</t>
+          <t>STX : 2015-10-01</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
@@ -6345,7 +6345,7 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>STX : 2015-10-01</t>
+          <t>SWN : 2015-10-01</t>
         </is>
       </c>
     </row>
@@ -6357,36 +6357,36 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>SWN : 2015-10-01</t>
+          <t>SWN : 2016-07-01</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>SWN : 2016-07-01</t>
+          <t>SYK : 2016-07-01</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
@@ -6396,14 +6396,14 @@
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>SYK : 2016-07-01</t>
+          <t>TDG : 2016-01-01</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>CCC</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
@@ -6413,7 +6413,7 @@
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>TDG : 2016-01-01</t>
+          <t>TEX : 2013-01-01</t>
         </is>
       </c>
     </row>
@@ -6430,14 +6430,14 @@
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>TEX : 2013-01-01</t>
+          <t>TEX : 2013-10-01</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
@@ -6447,7 +6447,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>TEX : 2013-10-01</t>
+          <t>TEX : 2016-04-01</t>
         </is>
       </c>
     </row>
@@ -6464,7 +6464,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>TEX : 2016-04-01</t>
+          <t>TGI : 2014-10-01</t>
         </is>
       </c>
     </row>
@@ -6481,7 +6481,7 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>TGI : 2014-10-01</t>
+          <t>TGI : 2015-01-01</t>
         </is>
       </c>
     </row>
@@ -6498,14 +6498,14 @@
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>TGI : 2015-01-01</t>
+          <t>TGNA : 2016-07-01</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
@@ -6515,7 +6515,7 @@
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>TGNA : 2016-07-01</t>
+          <t>TGT : 2013-07-01</t>
         </is>
       </c>
     </row>
@@ -6532,7 +6532,7 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>TGT : 2013-07-01</t>
+          <t>TGT : 2014-07-01</t>
         </is>
       </c>
     </row>
@@ -6549,7 +6549,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>TGT : 2014-07-01</t>
+          <t>TGT : 2014-10-01</t>
         </is>
       </c>
     </row>
@@ -6566,14 +6566,14 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>TGT : 2014-10-01</t>
+          <t>TGT : 2015-07-01</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
@@ -6583,31 +6583,31 @@
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>TGT : 2015-07-01</t>
+          <t>THC : 2012-07-01</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>THC : 2012-07-01</t>
+          <t>TKR : 2014-01-01</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
@@ -6617,7 +6617,7 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>TKR : 2014-01-01</t>
+          <t>TMUS : 2016-01-01</t>
         </is>
       </c>
     </row>
@@ -6634,7 +6634,7 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>TMUS : 2016-01-01</t>
+          <t>TMUS : 2016-07-01</t>
         </is>
       </c>
     </row>
@@ -6651,14 +6651,14 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>TMUS : 2016-07-01</t>
+          <t>TMUS : 2016-10-01</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -6668,14 +6668,14 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>TMUS : 2016-10-01</t>
+          <t>TOL : 2016-10-01</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
@@ -6685,14 +6685,14 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>TOL : 2016-10-01</t>
+          <t>TRMB : 2016-01-01</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -6702,7 +6702,7 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>TRMB : 2016-01-01</t>
+          <t>TRS : 2014-01-01</t>
         </is>
       </c>
     </row>
@@ -6719,14 +6719,14 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>TRS : 2014-01-01</t>
+          <t>TRS : 2016-10-01</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -6736,7 +6736,7 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>TRS : 2016-10-01</t>
+          <t>TUP : 2016-04-01</t>
         </is>
       </c>
     </row>
@@ -6753,14 +6753,14 @@
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>TUP : 2016-04-01</t>
+          <t>TUP : 2016-07-01</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -6770,7 +6770,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>TUP : 2016-07-01</t>
+          <t>TWI : 2014-01-01</t>
         </is>
       </c>
     </row>
@@ -6787,31 +6787,31 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>TWI : 2014-01-01</t>
+          <t>TWI : 2015-07-01</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>TWI : 2015-07-01</t>
+          <t>TXN : 2013-01-01</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
@@ -6821,7 +6821,7 @@
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>TXN : 2013-01-01</t>
+          <t>UHS : 2016-10-01</t>
         </is>
       </c>
     </row>
@@ -6833,12 +6833,12 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>UHS : 2016-10-01</t>
+          <t>UIS : 2013-10-01</t>
         </is>
       </c>
     </row>
@@ -6855,7 +6855,7 @@
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>UIS : 2013-10-01</t>
+          <t>UIS : 2014-07-01</t>
         </is>
       </c>
     </row>
@@ -6872,7 +6872,7 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>UIS : 2014-07-01</t>
+          <t>UIS : 2015-01-01</t>
         </is>
       </c>
     </row>
@@ -6884,12 +6884,12 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>UIS : 2015-01-01</t>
+          <t>UIS : 2015-04-01</t>
         </is>
       </c>
     </row>
@@ -6906,31 +6906,31 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>UIS : 2015-04-01</t>
+          <t>UIS : 2016-01-01</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>UIS : 2016-01-01</t>
+          <t>UPS : 2015-01-01</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -6940,31 +6940,31 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>UPS : 2015-01-01</t>
+          <t>URI : 2013-10-01</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>URI : 2013-10-01</t>
+          <t>USM : 2013-04-01</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
@@ -6974,14 +6974,14 @@
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>USM : 2013-04-01</t>
+          <t>USM : 2014-10-01</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
@@ -6991,14 +6991,14 @@
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>USM : 2014-10-01</t>
+          <t>VGR : 2014-10-01</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
@@ -7008,14 +7008,14 @@
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>VGR : 2014-10-01</t>
+          <t>VMC : 2014-01-01</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
@@ -7025,14 +7025,14 @@
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>VMC : 2014-01-01</t>
+          <t>VMI : 2014-10-01</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
@@ -7042,14 +7042,14 @@
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>VMI : 2014-10-01</t>
+          <t>VSH : 2014-10-01</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
@@ -7059,7 +7059,7 @@
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>VSH : 2014-10-01</t>
+          <t>WBA : 2013-07-01</t>
         </is>
       </c>
     </row>
@@ -7076,14 +7076,14 @@
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>WBA : 2013-07-01</t>
+          <t>WEC : 2015-10-01</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
@@ -7093,7 +7093,7 @@
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>WEC : 2015-10-01</t>
+          <t>WM : 2016-01-01</t>
         </is>
       </c>
     </row>
@@ -7110,14 +7110,14 @@
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>WM : 2016-01-01</t>
+          <t>WM : 2016-07-01</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
@@ -7127,14 +7127,14 @@
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>WM : 2016-07-01</t>
+          <t>WMB : 2013-07-01</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
@@ -7144,31 +7144,31 @@
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>WMB : 2013-07-01</t>
+          <t>WTI : 2014-01-01</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>WTI : 2014-01-01</t>
+          <t>XEL : 2013-10-01</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
@@ -7178,7 +7178,7 @@
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>XEL : 2013-10-01</t>
+          <t>XEL : 2016-01-01</t>
         </is>
       </c>
     </row>
@@ -7195,7 +7195,7 @@
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>XEL : 2016-01-01</t>
+          <t>XEL : 2016-07-01</t>
         </is>
       </c>
     </row>
@@ -7212,48 +7212,48 @@
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>XEL : 2016-07-01</t>
+          <t>XEL : 2016-10-01</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>AAA</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>XEL : 2016-10-01</t>
+          <t>XOM : 2016-01-01</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>AAA</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>XOM : 2016-01-01</t>
+          <t>YUM : 2015-04-01</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
@@ -7262,23 +7262,6 @@
         </is>
       </c>
       <c r="C402" t="inlineStr">
-        <is>
-          <t>YUM : 2015-04-01</t>
-        </is>
-      </c>
-    </row>
-    <row r="403">
-      <c r="A403" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="B403" t="inlineStr">
-        <is>
-          <t>BBB</t>
-        </is>
-      </c>
-      <c r="C403" t="inlineStr">
         <is>
           <t>ZBRA : 2016-10-01</t>
         </is>

</xml_diff>

<commit_message>
keep highest val strategy
</commit_message>
<xml_diff>
--- a/Data/Predictions/Graph Neural Network/Inductive/exclude_previous_rating_model_1_predictions.xlsx
+++ b/Data/Predictions/Graph Neural Network/Inductive/exclude_previous_rating_model_1_predictions.xlsx
@@ -662,7 +662,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2634,7 +2634,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3246,7 +3246,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -3348,7 +3348,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -3365,7 +3365,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -3382,7 +3382,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -4045,7 +4045,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -4079,7 +4079,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -4198,7 +4198,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -4215,7 +4215,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -5898,7 +5898,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -6357,7 +6357,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">

</xml_diff>